<commit_message>
upload de arquivo transferido para o react
</commit_message>
<xml_diff>
--- a/backend/certa.xlsx
+++ b/backend/certa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia\Desktop\api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\GitHub\Dashboard-Pro4Tech\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8666B53E-0602-4831-B71D-A2297E9FEC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC3F9CB-629B-4773-BEE7-8ED6C6B044DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="2775" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Data_da_venda</t>
   </si>
@@ -158,15 +158,25 @@
   </si>
   <si>
     <t>Segmento B</t>
+  </si>
+  <si>
+    <t>Gustavo Sena</t>
+  </si>
+  <si>
+    <t>11/04/2024</t>
+  </si>
+  <si>
+    <t>333.333.333-34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;R$&quot;\ #,##0;[Red]\-&quot;R$&quot;\ #,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -209,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,6 +255,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,10 +507,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,6 +720,41 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -714,6 +762,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FF33F66F804B4D49AAA3ACD3A2BB6BED" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2963f910d82ea0d582049579ebaab953">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b27184c-fad0-44bf-8a16-f94ff7fe2173" xmlns:ns3="292518d5-5be3-4e47-a7a5-bd650e8326a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2580e056891786b547c963399f6d2401" ns2:_="" ns3:_="">
     <xsd:import namespace="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
@@ -942,15 +999,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -963,13 +1011,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382F5758-AFBC-4D1B-9183-6D9DDB472913}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F63929-21AA-4D9C-988E-3E66BB7E53BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F63929-21AA-4D9C-988E-3E66BB7E53BA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382F5758-AFBC-4D1B-9183-6D9DDB472913}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
+    <ds:schemaRef ds:uri="292518d5-5be3-4e47-a7a5-bd650e8326a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D8C745B-C62D-4376-8799-6B253189ACDE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D8C745B-C62D-4376-8799-6B253189ACDE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="292518d5-5be3-4e47-a7a5-bd650e8326a1"/>
+    <ds:schemaRef ds:uri="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adição da planilha atual
</commit_message>
<xml_diff>
--- a/backend/certa.xlsx
+++ b/backend/certa.xlsx
@@ -1,26 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\GitHub\Dashboard-Pro4Tech\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedrinho\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC3F9CB-629B-4773-BEE7-8ED6C6B044DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{4BCCC6E2-120F-44FF-9B96-29AF76C2AE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E4253A-54FE-442F-95F2-2B5287D43F54}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>Data_da_venda</t>
   </si>
@@ -55,7 +74,7 @@
     <t>Rafael Araújo Moreno Monteiro</t>
   </si>
   <si>
-    <t>123.456.789-00</t>
+    <t>000.000.000-00</t>
   </si>
   <si>
     <t>Sistema de descrição de cargos</t>
@@ -76,113 +95,145 @@
     <t>Dianne Faria</t>
   </si>
   <si>
-    <t>000.000.000-00</t>
-  </si>
-  <si>
-    <t>Escola</t>
-  </si>
-  <si>
-    <t>00.000.000/0000-00</t>
-  </si>
-  <si>
-    <t>Aula</t>
+    <t>111.111.111-11</t>
+  </si>
+  <si>
+    <t>Sistema organizador de matéria</t>
+  </si>
+  <si>
+    <t>Leonardo Mendes</t>
+  </si>
+  <si>
+    <t>71.589.249/5491-20</t>
+  </si>
+  <si>
+    <t>Escolar</t>
   </si>
   <si>
     <t>Á vista</t>
   </si>
   <si>
-    <t>111.111.111-11</t>
-  </si>
-  <si>
-    <t>Pessoa</t>
-  </si>
-  <si>
-    <t>11.111.111/1111-11</t>
-  </si>
-  <si>
-    <t>Jogo</t>
+    <t>Marcos Antônio</t>
   </si>
   <si>
     <t>222.222.222-22</t>
   </si>
   <si>
-    <t>pessoa1</t>
+    <t>Aplicativo Empresarial</t>
+  </si>
+  <si>
+    <t>Amanda Lima</t>
+  </si>
+  <si>
+    <t>52.489.294/3295-20</t>
+  </si>
+  <si>
+    <t>Saúde</t>
+  </si>
+  <si>
+    <t>Claudio Gomes</t>
+  </si>
+  <si>
+    <t>333.333.333-33</t>
+  </si>
+  <si>
+    <t>Plataforma E-commerce</t>
+  </si>
+  <si>
+    <t>Jean Santos</t>
   </si>
   <si>
     <t>22.222.222/2222-22</t>
   </si>
   <si>
-    <t>222.222.222-23</t>
-  </si>
-  <si>
-    <t>22.222.222/2222-23</t>
-  </si>
-  <si>
-    <t>10/01/2024</t>
-  </si>
-  <si>
-    <t>15/07/2024</t>
-  </si>
-  <si>
-    <t>11/11/2024</t>
-  </si>
-  <si>
-    <t>27/12/2024</t>
-  </si>
-  <si>
-    <t>10/04/2024</t>
-  </si>
-  <si>
-    <t>Marcos Antônio</t>
-  </si>
-  <si>
-    <t>Claudio Gomes</t>
+    <t>Vestuário</t>
   </si>
   <si>
     <t>Brenda Lopes</t>
   </si>
   <si>
-    <t>Produto A</t>
-  </si>
-  <si>
-    <t>Produto E</t>
-  </si>
-  <si>
-    <t>Produto B</t>
-  </si>
-  <si>
-    <t>Pessoa2</t>
-  </si>
-  <si>
-    <t>Segmento A</t>
-  </si>
-  <si>
-    <t>Segmento B</t>
+    <t>444.444.444-44</t>
+  </si>
+  <si>
+    <t>Aplicativo Mobile</t>
+  </si>
+  <si>
+    <t>Lívia Oliveira</t>
+  </si>
+  <si>
+    <t>16.589.952/2560-01</t>
+  </si>
+  <si>
+    <t>Automotivo</t>
+  </si>
+  <si>
+    <t>Thais Costa</t>
+  </si>
+  <si>
+    <t>555.555.555-55</t>
+  </si>
+  <si>
+    <t>Sistema de Gerenciamento</t>
+  </si>
+  <si>
+    <t>Beatriz Costa</t>
+  </si>
+  <si>
+    <t>75.289.522/7382-87</t>
+  </si>
+  <si>
+    <t>Administrativo</t>
+  </si>
+  <si>
+    <t>Diego Garcia</t>
+  </si>
+  <si>
+    <t>55.525.521/7731-12</t>
+  </si>
+  <si>
+    <t>Startup</t>
+  </si>
+  <si>
+    <t>Alimentício</t>
+  </si>
+  <si>
+    <t>Aplicativo de Saúde</t>
+  </si>
+  <si>
+    <t>Software de RH</t>
   </si>
   <si>
     <t>Gustavo Sena</t>
   </si>
   <si>
-    <t>11/04/2024</t>
-  </si>
-  <si>
-    <t>333.333.333-34</t>
+    <t>32.067.321/0001-50</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>Sistema de Gestão de Projetos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;R$&quot;\ #,##0;[Red]\-&quot;R$&quot;\ #,##0"/>
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -192,8 +243,20 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Söhne Mono"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +267,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor theme="5" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -219,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,31 +302,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,32 +582,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" style="3" customWidth="1"/>
-    <col min="11" max="24" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="25" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="15.75">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -541,219 +616,517 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14">
+        <v>45301</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2">
         <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="12">
         <v>1500</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="K2" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14">
+        <v>45488</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="12">
+        <v>1000.5</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14">
+        <v>45607</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1950</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>45653</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="12">
+        <v>3000</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
+        <v>45392</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1200</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>45422</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="12">
+        <v>2500</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14">
+        <v>45537</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1650</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14">
+        <v>45327</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="12">
+        <v>2100</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>45534</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="12">
+        <v>2880</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14">
+        <v>111111</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="11">
-        <v>1000.5</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="12">
+        <v>2300</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14">
+        <v>45342</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2">
+        <v>7</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="12">
+        <v>4000</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14">
+        <v>45458</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1950</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14">
+        <v>45567</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="12">
+        <v>4500</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="12">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3" t="s">
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14">
+        <v>45567</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="12">
-        <v>15</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="12">
-        <v>20</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I8" s="14"/>
+      <c r="J15" s="12">
+        <v>2500</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
@@ -762,6 +1135,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="292518d5-5be3-4e47-a7a5-bd650e8326a1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b27184c-fad0-44bf-8a16-f94ff7fe2173">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -770,7 +1154,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FF33F66F804B4D49AAA3ACD3A2BB6BED" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2963f910d82ea0d582049579ebaab953">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b27184c-fad0-44bf-8a16-f94ff7fe2173" xmlns:ns3="292518d5-5be3-4e47-a7a5-bd650e8326a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2580e056891786b547c963399f6d2401" ns2:_="" ns3:_="">
     <xsd:import namespace="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
@@ -999,51 +1383,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="292518d5-5be3-4e47-a7a5-bd650e8326a1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b27184c-fad0-44bf-8a16-f94ff7fe2173">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F63929-21AA-4D9C-988E-3E66BB7E53BA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D8C745B-C62D-4376-8799-6B253189ACDE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382F5758-AFBC-4D1B-9183-6D9DDB472913}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
-    <ds:schemaRef ds:uri="292518d5-5be3-4e47-a7a5-bd650e8326a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F63929-21AA-4D9C-988E-3E66BB7E53BA}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D8C745B-C62D-4376-8799-6B253189ACDE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="292518d5-5be3-4e47-a7a5-bd650e8326a1"/>
-    <ds:schemaRef ds:uri="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382F5758-AFBC-4D1B-9183-6D9DDB472913}"/>
 </file>
</xml_diff>

<commit_message>
1° parte da visao de vendedor
</commit_message>
<xml_diff>
--- a/backend/certa.xlsx
+++ b/backend/certa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedrinho\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\GitHub\Dashboard-Pro4Tech\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{4BCCC6E2-120F-44FF-9B96-29AF76C2AE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E4253A-54FE-442F-95F2-2B5287D43F54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4FA0C3-B5DD-4CA2-99A7-D5254D8A3CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Sistema de Gestão de Projetos</t>
+  </si>
+  <si>
+    <t>Gustavo Pessoa</t>
+  </si>
+  <si>
+    <t>433.534.428-72</t>
   </si>
 </sst>
 </file>
@@ -222,11 +228,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -288,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,38 +315,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +596,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -937,7 +951,7 @@
       <c r="F10" s="2">
         <v>4</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="19" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -1125,6 +1139,146 @@
         <v>2500</v>
       </c>
       <c r="K15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14">
+        <v>45607</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="2">
+        <v>6</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="12">
+        <v>2500</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14">
+        <v>111111</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="2">
+        <v>9</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="12">
+        <v>2500</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14">
+        <v>45392</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="2">
+        <v>4</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="12">
+        <v>2880</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="12">
+        <v>1000.5</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1135,6 +1289,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="292518d5-5be3-4e47-a7a5-bd650e8326a1" xsi:nil="true"/>
@@ -1143,15 +1306,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1384,13 +1538,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D8C745B-C62D-4376-8799-6B253189ACDE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F63929-21AA-4D9C-988E-3E66BB7E53BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F63929-21AA-4D9C-988E-3E66BB7E53BA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D8C745B-C62D-4376-8799-6B253189ACDE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="292518d5-5be3-4e47-a7a5-bd650e8326a1"/>
+    <ds:schemaRef ds:uri="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382F5758-AFBC-4D1B-9183-6D9DDB472913}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{382F5758-AFBC-4D1B-9183-6D9DDB472913}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b27184c-fad0-44bf-8a16-f94ff7fe2173"/>
+    <ds:schemaRef ds:uri="292518d5-5be3-4e47-a7a5-bd650e8326a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>